<commit_message>
Updating PCA to include underoccupation and possession claims.
</commit_message>
<xml_diff>
--- a/20250815_dataset_guide_MM_V1.xlsx
+++ b/20250815_dataset_guide_MM_V1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\marshall_group\User\gp1mmx\housing_populism\data\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\marshall_group\User\gp1mmx\housing_populism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3E2A28-F755-4A0D-B235-95393A233D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2316B685-0756-4436-81B7-DDF7FD32AF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5FF58C6B-ED44-4846-AD90-2C48070ED693}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
   <si>
     <t>Dataset</t>
   </si>
@@ -309,6 +309,24 @@
   </si>
   <si>
     <t>https://www.britishelectionstudy.com/data-objects/panel-study-data/</t>
+  </si>
+  <si>
+    <t>Landlord possession claims</t>
+  </si>
+  <si>
+    <t>possession_statistics_2024</t>
+  </si>
+  <si>
+    <t>MAP_CSV</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/media/66b360d9a3c2a28abb50de35/Mortgage_and_landlord_statistical_data.zip</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/media/620397bce90e077f71cd545b/Mortgage_and_landlord_statistical_data.zip</t>
+  </si>
+  <si>
+    <t>possession_statistics_2021</t>
   </si>
 </sst>
 </file>
@@ -685,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6046FEFF-7B6C-4C9D-8A89-917581189BF4}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1311,52 @@
         <v>90</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F27" s="1">
+        <v>45902</v>
+      </c>
+      <c r="G27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2021</v>
+      </c>
+      <c r="F28" s="1">
+        <v>45902</v>
+      </c>
+      <c r="G28" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G21">
     <sortCondition ref="B2:B21"/>

</xml_diff>